<commit_message>
Changes for final video and streamingAsset configuration
</commit_message>
<xml_diff>
--- a/ExcelFiles/Example_ExcelSheet.xlsx
+++ b/ExcelFiles/Example_ExcelSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivian\OneDrive\Desktop\Lightsaber-Innoprojekt\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e501a7a985e1327d/Desktop/Lightsaber-Innoprojekt/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9954E001-DA64-43E9-8D86-D2BECF0BCF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{9954E001-DA64-43E9-8D86-D2BECF0BCF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B14CC0C5-9926-4D60-B4A7-A152751166AF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{846AA384-759E-4EAF-B295-246274DCC9D7}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Sentence</t>
   </si>
@@ -67,25 +67,19 @@
     <t>correctBlock</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>test4</t>
-  </si>
-  <si>
-    <t>Example sentence</t>
-  </si>
-  <si>
-    <t>Second example</t>
-  </si>
-  <si>
-    <t>…</t>
+    <t>This is a  ___ sentence</t>
+  </si>
+  <si>
+    <t>false1</t>
+  </si>
+  <si>
+    <t>false2</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>false3</t>
   </si>
 </sst>
 </file>
@@ -127,10 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -198,11 +191,15 @@
 </MapInfo>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{6286A987-ADEC-4822-AECA-279BCF200BE1}" name="Tabelle12" displayName="Tabelle12" ref="A1:F5" tableType="xml" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{6286A987-ADEC-4822-AECA-279BCF200BE1}" name="Tabelle12" displayName="Tabelle12" ref="A1:F5" tableType="xml" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:F5" xr:uid="{6286A987-ADEC-4822-AECA-279BCF200BE1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9F17715D-4393-47CF-A3CB-193572478A6B}" uniqueName="Sentence" name="Sentence" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{9F17715D-4393-47CF-A3CB-193572478A6B}" uniqueName="Sentence" name="Sentence" dataDxfId="5">
       <xmlColumnPr mapId="4" xpath="/Level/LevelPart/Sentence" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{0B897AC3-5A66-40FD-AB97-2E1D718B3AB2}" uniqueName="Block1" name="Block1" dataDxfId="4">
@@ -525,7 +522,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -560,83 +557,46 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2">
-        <v>123</v>
+      <c r="F2">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="2">
-        <v>456</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>

</xml_diff>